<commit_message>
update câu hỏi giải đáp yêu của khách hàng
</commit_message>
<xml_diff>
--- a/2015/201512/30_Q&A/Q&A.xlsx
+++ b/2015/201512/30_Q&A/Q&A.xlsx
@@ -98,9 +98,6 @@
     <t>Thị Phượng</t>
   </si>
   <si>
-    <t>Hoàng Vũ</t>
-  </si>
-  <si>
     <t>Module T</t>
   </si>
   <si>
@@ -110,12 +107,15 @@
     <t>Chọn đề xuất</t>
   </si>
   <si>
+    <t>Hoàng Vũ, Phát Danh</t>
+  </si>
+  <si>
     <t>- Hiện trạng: theo yêu cầu của Customize Hoàng Trần sẽ tạo thêm màn hình Xác nhận thủ quỹ - AF0324 để quét mã vạch thủ quỹ  và được gắn link tại Module T
-- Vấn đề: Nơi đặt màn hình Xác nhận Thủ quỹ trong Module T
+- Vấn đề: Nơi đặt màn hình Xác nhận thủ quỹ - AF0324trong Module T
 - Đề xuất:  
   + Đề xuất 1: Tại Nghiệp vụ tạo thêm mục M Barcode Quỹ 
   + Đề xuất 2: Tại Danh mục tạo thêm mục K Barcode Quỹ 
-  + Đề xuất 3: Tại Nghiệp vu -&gt; Tiền tại quỹ tạo thêm mục 5 Barcode Quỹ</t>
+  + Đề xuất 3: Tại Nghiệp vụ -&gt; Tiền tại quỹ tạo thêm mục 5 Barcode Quỹ</t>
   </si>
 </sst>
 </file>
@@ -704,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="12.75"/>
@@ -823,14 +823,14 @@
         <v>22</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="29"/>
       <c r="F3" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="31" t="s">
         <v>26</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>27</v>
       </c>
       <c r="H3" s="32">
         <v>42383</v>
@@ -842,7 +842,7 @@
         <v>28</v>
       </c>
       <c r="L3" s="33" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M3" s="34">
         <v>42383</v>

</xml_diff>